<commit_message>
updated datafiles row +10
</commit_message>
<xml_diff>
--- a/Excel/7. DataFile_NAP_CF4W_Company.xlsx
+++ b/Excel/7. DataFile_NAP_CF4W_Company.xlsx
@@ -5,11 +5,11 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jeremy.andreas\git\NAP-CF4W-UF-New\Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fendy.tio\git\NAP-CF4W-UFNEW\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15705" windowHeight="5820" tabRatio="769" firstSheet="15" activeTab="18"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15705" windowHeight="5820" tabRatio="769" firstSheet="15" activeTab="15"/>
   </bookViews>
   <sheets>
     <sheet name="0.Setting" sheetId="5" r:id="rId1"/>
@@ -34,7 +34,6 @@
   </sheets>
   <externalReferences>
     <externalReference r:id="rId20"/>
-    <externalReference r:id="rId21"/>
   </externalReferences>
   <definedNames>
     <definedName name="ExternalData_1" localSheetId="18" hidden="1">Master!$A$1:$B$43</definedName>
@@ -14213,6 +14212,17 @@
     <xf numFmtId="0" fontId="9" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -14245,17 +14255,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -21071,19 +21070,6 @@
           </cell>
         </row>
       </sheetData>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
-<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Master"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -22816,13 +22802,13 @@
     <row r="9" spans="1:5" s="17" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="10" spans="1:5" s="17" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="11" spans="1:5" s="102" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="121" t="s">
+      <c r="A11" s="109" t="s">
         <v>3163</v>
       </c>
-      <c r="B11" s="122"/>
-      <c r="C11" s="122"/>
-      <c r="D11" s="122"/>
-      <c r="E11" s="123"/>
+      <c r="B11" s="110"/>
+      <c r="C11" s="110"/>
+      <c r="D11" s="110"/>
+      <c r="E11" s="111"/>
     </row>
     <row r="12" spans="1:5" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="50" t="s">
@@ -22832,14 +22818,14 @@
         <v>192</v>
       </c>
     </row>
-    <row r="13" spans="1:5" s="125" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="119" t="s">
+    <row r="13" spans="1:5" s="113" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="107" t="s">
         <v>91</v>
       </c>
-      <c r="B13" s="120"/>
-      <c r="C13" s="120"/>
-      <c r="D13" s="120"/>
-      <c r="E13" s="124"/>
+      <c r="B13" s="108"/>
+      <c r="C13" s="108"/>
+      <c r="D13" s="108"/>
+      <c r="E13" s="112"/>
     </row>
     <row r="14" spans="1:5" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="51" t="s">
@@ -22888,14 +22874,14 @@
         <v>199</v>
       </c>
     </row>
-    <row r="21" spans="1:5" s="125" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="119" t="s">
+    <row r="21" spans="1:5" s="113" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="107" t="s">
         <v>81</v>
       </c>
-      <c r="B21" s="120"/>
-      <c r="C21" s="120"/>
-      <c r="D21" s="120"/>
-      <c r="E21" s="124"/>
+      <c r="B21" s="108"/>
+      <c r="C21" s="108"/>
+      <c r="D21" s="108"/>
+      <c r="E21" s="112"/>
     </row>
     <row r="22" spans="1:5" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="51" t="s">
@@ -22951,13 +22937,13 @@
       </c>
     </row>
     <row r="29" spans="1:5" s="102" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="121" t="s">
+      <c r="A29" s="109" t="s">
         <v>3164</v>
       </c>
-      <c r="B29" s="122"/>
-      <c r="C29" s="122"/>
-      <c r="D29" s="122"/>
-      <c r="E29" s="123"/>
+      <c r="B29" s="110"/>
+      <c r="C29" s="110"/>
+      <c r="D29" s="110"/>
+      <c r="E29" s="111"/>
     </row>
     <row r="30" spans="1:5" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="54" t="s">
@@ -22983,14 +22969,14 @@
         <v>800000</v>
       </c>
     </row>
-    <row r="33" spans="1:5" s="129" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="126" t="s">
+    <row r="33" spans="1:5" s="117" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="114" t="s">
         <v>3165</v>
       </c>
-      <c r="B33" s="127"/>
-      <c r="C33" s="127"/>
-      <c r="D33" s="127"/>
-      <c r="E33" s="128"/>
+      <c r="B33" s="115"/>
+      <c r="C33" s="115"/>
+      <c r="D33" s="115"/>
+      <c r="E33" s="116"/>
     </row>
     <row r="34" spans="1:5" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="51" t="s">
@@ -23000,14 +22986,14 @@
         <v>212</v>
       </c>
     </row>
-    <row r="35" spans="1:5" s="119" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="119" t="s">
+    <row r="35" spans="1:5" s="107" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="107" t="s">
         <v>213</v>
       </c>
-      <c r="B35" s="120"/>
-      <c r="C35" s="120"/>
-      <c r="D35" s="120"/>
-      <c r="E35" s="120"/>
+      <c r="B35" s="108"/>
+      <c r="C35" s="108"/>
+      <c r="D35" s="108"/>
+      <c r="E35" s="108"/>
     </row>
     <row r="36" spans="1:5" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="17" t="s">
@@ -23076,14 +23062,14 @@
       <c r="D43" s="92"/>
       <c r="E43" s="92"/>
     </row>
-    <row r="44" spans="1:5" s="108" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="108" t="s">
+    <row r="44" spans="1:5" s="119" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="119" t="s">
         <v>3351</v>
       </c>
-      <c r="B44" s="109"/>
-      <c r="C44" s="109"/>
-      <c r="D44" s="109"/>
-      <c r="E44" s="109"/>
+      <c r="B44" s="120"/>
+      <c r="C44" s="120"/>
+      <c r="D44" s="120"/>
+      <c r="E44" s="120"/>
     </row>
     <row r="45" spans="1:5" s="76" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="76" t="s">
@@ -23117,14 +23103,14 @@
         <v>3449</v>
       </c>
     </row>
-    <row r="49" spans="1:5" s="110" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="110" t="s">
+    <row r="49" spans="1:5" s="121" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="121" t="s">
         <v>213</v>
       </c>
-      <c r="B49" s="111"/>
-      <c r="C49" s="111"/>
-      <c r="D49" s="111"/>
-      <c r="E49" s="111"/>
+      <c r="B49" s="122"/>
+      <c r="C49" s="122"/>
+      <c r="D49" s="122"/>
+      <c r="E49" s="122"/>
     </row>
     <row r="50" spans="1:5" s="76" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" s="76" t="s">
@@ -23190,8 +23176,8 @@
         <v>3453</v>
       </c>
     </row>
-    <row r="58" spans="1:5" s="112" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="112" t="s">
+    <row r="58" spans="1:5" s="123" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="123" t="s">
         <v>3337</v>
       </c>
     </row>
@@ -23353,11 +23339,11 @@
       </c>
       <c r="B79" s="11"/>
     </row>
-    <row r="80" spans="1:2" s="113" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="113" t="s">
+    <row r="80" spans="1:2" s="124" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A80" s="124" t="s">
         <v>3166</v>
       </c>
-      <c r="B80" s="114"/>
+      <c r="B80" s="125"/>
     </row>
     <row r="81" spans="1:2" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A81" s="17" t="s">
@@ -23376,10 +23362,10 @@
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A84" s="115" t="s">
+      <c r="A84" s="126" t="s">
         <v>3346</v>
       </c>
-      <c r="B84" s="116"/>
+      <c r="B84" s="127"/>
     </row>
     <row r="85" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A85" s="82" t="s">
@@ -23391,10 +23377,10 @@
       </c>
     </row>
     <row r="86" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="117" t="s">
+      <c r="A86" s="128" t="s">
         <v>3345</v>
       </c>
-      <c r="B86" s="118"/>
+      <c r="B86" s="129"/>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" s="75" t="s">
@@ -23406,23 +23392,17 @@
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A88" s="107" t="s">
+      <c r="A88" s="118" t="s">
         <v>3352</v>
       </c>
-      <c r="B88" s="107"/>
+      <c r="B88" s="118"/>
     </row>
     <row r="89" spans="1:2" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A89" s="107"/>
-      <c r="B89" s="107"/>
+      <c r="A89" s="118"/>
+      <c r="B89" s="118"/>
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A35:XFD35"/>
-    <mergeCell ref="A11:XFD11"/>
-    <mergeCell ref="A13:XFD13"/>
-    <mergeCell ref="A21:XFD21"/>
-    <mergeCell ref="A29:XFD29"/>
-    <mergeCell ref="A33:XFD33"/>
     <mergeCell ref="A88:B89"/>
     <mergeCell ref="A44:XFD44"/>
     <mergeCell ref="A49:XFD49"/>
@@ -23430,6 +23410,12 @@
     <mergeCell ref="A80:XFD80"/>
     <mergeCell ref="A84:B84"/>
     <mergeCell ref="A86:B86"/>
+    <mergeCell ref="A35:XFD35"/>
+    <mergeCell ref="A11:XFD11"/>
+    <mergeCell ref="A13:XFD13"/>
+    <mergeCell ref="A21:XFD21"/>
+    <mergeCell ref="A29:XFD29"/>
+    <mergeCell ref="A33:XFD33"/>
   </mergeCells>
   <conditionalFormatting sqref="A28:XFD28">
     <cfRule type="expression" dxfId="91" priority="8">
@@ -23833,13 +23819,13 @@
     <row r="9" spans="1:5" s="17" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="10" spans="1:5" s="17" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="11" spans="1:5" s="102" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="121" t="s">
+      <c r="A11" s="109" t="s">
         <v>3170</v>
       </c>
-      <c r="B11" s="122"/>
-      <c r="C11" s="122"/>
-      <c r="D11" s="122"/>
-      <c r="E11" s="123"/>
+      <c r="B11" s="110"/>
+      <c r="C11" s="110"/>
+      <c r="D11" s="110"/>
+      <c r="E11" s="111"/>
     </row>
     <row r="12" spans="1:5" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="55" t="s">
@@ -23891,14 +23877,14 @@
         <v>242</v>
       </c>
     </row>
-    <row r="19" spans="1:5" s="121" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="121" t="s">
+    <row r="19" spans="1:5" s="109" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="109" t="s">
         <v>3171</v>
       </c>
-      <c r="B19" s="122"/>
-      <c r="C19" s="122"/>
-      <c r="D19" s="122"/>
-      <c r="E19" s="122"/>
+      <c r="B19" s="110"/>
+      <c r="C19" s="110"/>
+      <c r="D19" s="110"/>
+      <c r="E19" s="110"/>
     </row>
     <row r="20" spans="1:5" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="49" t="s">
@@ -24076,14 +24062,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:5" s="121" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="121" t="s">
+    <row r="42" spans="1:5" s="109" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="109" t="s">
         <v>3172</v>
       </c>
-      <c r="B42" s="122"/>
-      <c r="C42" s="122"/>
-      <c r="D42" s="122"/>
-      <c r="E42" s="122"/>
+      <c r="B42" s="110"/>
+      <c r="C42" s="110"/>
+      <c r="D42" s="110"/>
+      <c r="E42" s="110"/>
     </row>
     <row r="43" spans="1:5" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="17" t="s">
@@ -24615,7 +24601,7 @@
   <sheetPr codeName="Sheet16"/>
   <dimension ref="A1:E57"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="A2" sqref="A2:A3"/>
     </sheetView>
@@ -24673,12 +24659,12 @@
       </c>
     </row>
     <row r="13" spans="1:5" s="132" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="113" t="s">
+      <c r="A13" s="124" t="s">
         <v>2564</v>
       </c>
-      <c r="B13" s="114"/>
-      <c r="C13" s="114"/>
-      <c r="D13" s="114"/>
+      <c r="B13" s="125"/>
+      <c r="C13" s="125"/>
+      <c r="D13" s="125"/>
       <c r="E13" s="131"/>
     </row>
     <row r="14" spans="1:5" s="17" customFormat="1" x14ac:dyDescent="0.25">
@@ -24776,12 +24762,12 @@
       </c>
     </row>
     <row r="26" spans="1:5" s="132" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="113" t="s">
+      <c r="A26" s="124" t="s">
         <v>2568</v>
       </c>
-      <c r="B26" s="114"/>
-      <c r="C26" s="114"/>
-      <c r="D26" s="114"/>
+      <c r="B26" s="125"/>
+      <c r="C26" s="125"/>
+      <c r="D26" s="125"/>
       <c r="E26" s="131"/>
     </row>
     <row r="27" spans="1:5" s="17" customFormat="1" x14ac:dyDescent="0.25">
@@ -24901,10 +24887,10 @@
       </c>
     </row>
     <row r="42" spans="1:2" s="132" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="113" t="s">
+      <c r="A42" s="124" t="s">
         <v>2552</v>
       </c>
-      <c r="B42" s="114"/>
+      <c r="B42" s="125"/>
     </row>
     <row r="43" spans="1:2" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="17" t="s">
@@ -25292,7 +25278,7 @@
   <sheetPr codeName="Sheet19"/>
   <dimension ref="A1:DS492"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="DP1" workbookViewId="0">
+    <sheetView topLeftCell="DP1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="DS9" sqref="DS9"/>
     </sheetView>

</xml_diff>